<commit_message>
fix report for 2. auffr
</commit_message>
<xml_diff>
--- a/data/kbvreport_export/faktenblatttabellen_2022-02-27.xlsx
+++ b/data/kbvreport_export/faktenblatttabellen_2022-02-27.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="414">
   <si>
     <t xml:space="preserve">Geimpfte Personen</t>
   </si>
@@ -30,7 +30,7 @@
     <t xml:space="preserve">Vorwoche</t>
   </si>
   <si>
-    <t xml:space="preserve">Stand 3.3.</t>
+    <t xml:space="preserve">Stand 4.3.</t>
   </si>
   <si>
     <t xml:space="preserve">Anteil_Veraenderung</t>
@@ -45,10 +45,10 @@
     <t xml:space="preserve">Gesamt</t>
   </si>
   <si>
-    <t xml:space="preserve">63416464 (76,3 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">63479876 (76,3 %)</t>
+    <t xml:space="preserve">63428909 (76,3 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">63492423 (76,3 %)</t>
   </si>
   <si>
     <t xml:space="preserve"> 0,1 PP</t>
@@ -57,10 +57,10 @@
     <t xml:space="preserve">Nicht vollst. geimpft</t>
   </si>
   <si>
-    <t xml:space="preserve">810260 ( 1,0 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">704423 ( 0,8 %)</t>
+    <t xml:space="preserve">783765 ( 0,9 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">685933 ( 0,8 %)</t>
   </si>
   <si>
     <t xml:space="preserve">-0,1 PP</t>
@@ -69,10 +69,10 @@
     <t xml:space="preserve">Vollst. geimpft</t>
   </si>
   <si>
-    <t xml:space="preserve">62606204 (75,3 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">62775453 (75,5 %)</t>
+    <t xml:space="preserve">62645144 (75,3 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">62806490 (75,5 %)</t>
   </si>
   <si>
     <t xml:space="preserve"> 0,2 PP</t>
@@ -81,10 +81,10 @@
     <t xml:space="preserve">Zusätzl. Booster-Impfung</t>
   </si>
   <si>
-    <t xml:space="preserve">47081705 (56,6 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">47529008 (57,1 %)</t>
+    <t xml:space="preserve">47189282 (56,7 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">47627669 (57,3 %)</t>
   </si>
   <si>
     <t xml:space="preserve"> 0,5 PP</t>
@@ -93,6 +93,12 @@
     <t xml:space="preserve">Zusätzl. 2. Booster-Impfung</t>
   </si>
   <si>
+    <t xml:space="preserve">317181 ( 0,4 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">516033 ( 0,6 %)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Impffortschritt</t>
   </si>
   <si>
@@ -165,13 +171,13 @@
     <t xml:space="preserve">7-Tage-Inzidenz 60+</t>
   </si>
   <si>
-    <t xml:space="preserve">76,3</t>
+    <t xml:space="preserve">76,4</t>
   </si>
   <si>
     <t xml:space="preserve">75,5</t>
   </si>
   <si>
-    <t xml:space="preserve">57,1</t>
+    <t xml:space="preserve">57,3</t>
   </si>
   <si>
     <t xml:space="preserve">Baden-Württemberg</t>
@@ -189,7 +195,7 @@
     <t xml:space="preserve">73,9</t>
   </si>
   <si>
-    <t xml:space="preserve">74,4</t>
+    <t xml:space="preserve">74,5</t>
   </si>
   <si>
     <t xml:space="preserve">55,0</t>
@@ -204,7 +210,7 @@
     <t xml:space="preserve">76,5</t>
   </si>
   <si>
-    <t xml:space="preserve">58,2</t>
+    <t xml:space="preserve">58,3</t>
   </si>
   <si>
     <t xml:space="preserve">Brandenburg</t>
@@ -216,7 +222,7 @@
     <t xml:space="preserve">68,9</t>
   </si>
   <si>
-    <t xml:space="preserve">50,6</t>
+    <t xml:space="preserve">50,7</t>
   </si>
   <si>
     <t xml:space="preserve">Bremen</t>
@@ -228,16 +234,16 @@
     <t xml:space="preserve">88,5</t>
   </si>
   <si>
-    <t xml:space="preserve">63,2</t>
+    <t xml:space="preserve">63,3</t>
   </si>
   <si>
     <t xml:space="preserve">Hamburg</t>
   </si>
   <si>
-    <t xml:space="preserve">82,9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">82,5</t>
+    <t xml:space="preserve">83,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">82,6</t>
   </si>
   <si>
     <t xml:space="preserve">Hessen</t>
@@ -249,16 +255,19 @@
     <t xml:space="preserve">74,2</t>
   </si>
   <si>
+    <t xml:space="preserve">55,1</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mecklenburg-Vorpommern</t>
   </si>
   <si>
     <t xml:space="preserve">74,3</t>
   </si>
   <si>
-    <t xml:space="preserve">74,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">55,3</t>
+    <t xml:space="preserve">74,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">55,5</t>
   </si>
   <si>
     <t xml:space="preserve">Niedersachsen</t>
@@ -267,10 +276,7 @@
     <t xml:space="preserve">78,3</t>
   </si>
   <si>
-    <t xml:space="preserve">77,2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">61,8</t>
+    <t xml:space="preserve">62,0</t>
   </si>
   <si>
     <t xml:space="preserve">Nordrhein-Westfalen</t>
@@ -282,19 +288,19 @@
     <t xml:space="preserve">78,4</t>
   </si>
   <si>
-    <t xml:space="preserve">59,6</t>
+    <t xml:space="preserve">59,8</t>
   </si>
   <si>
     <t xml:space="preserve">Rheinland-Pfalz</t>
   </si>
   <si>
-    <t xml:space="preserve">77,4</t>
+    <t xml:space="preserve">77,5</t>
   </si>
   <si>
     <t xml:space="preserve">74,7</t>
   </si>
   <si>
-    <t xml:space="preserve">57,5</t>
+    <t xml:space="preserve">57,6</t>
   </si>
   <si>
     <t xml:space="preserve">Saarland</t>
@@ -303,22 +309,22 @@
     <t xml:space="preserve">82,1</t>
   </si>
   <si>
-    <t xml:space="preserve">81,5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">64,2</t>
+    <t xml:space="preserve">81,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">64,3</t>
   </si>
   <si>
     <t xml:space="preserve">Sachsen</t>
   </si>
   <si>
-    <t xml:space="preserve">64,9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">63,8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">46,3</t>
+    <t xml:space="preserve">65,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">63,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">46,5</t>
   </si>
   <si>
     <t xml:space="preserve">Sachsen-Anhalt</t>
@@ -330,7 +336,7 @@
     <t xml:space="preserve">72,2</t>
   </si>
   <si>
-    <t xml:space="preserve">52,2</t>
+    <t xml:space="preserve">52,3</t>
   </si>
   <si>
     <t xml:space="preserve">Schleswig-Holstein</t>
@@ -339,19 +345,19 @@
     <t xml:space="preserve">80,5</t>
   </si>
   <si>
-    <t xml:space="preserve">80,4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">67,9</t>
+    <t xml:space="preserve">68,2</t>
   </si>
   <si>
     <t xml:space="preserve">Thüringen</t>
   </si>
   <si>
-    <t xml:space="preserve">69,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50,0</t>
+    <t xml:space="preserve">69,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">69,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50,1</t>
   </si>
   <si>
     <t xml:space="preserve">Impfstoffdosen</t>
@@ -363,42 +369,48 @@
     <t xml:space="preserve">Biontech/Pfizer</t>
   </si>
   <si>
-    <t xml:space="preserve">124038705 (73,2 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">124606816 (73,2 %)</t>
+    <t xml:space="preserve">124416278 (73,2 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">125123494 (73,2 %)</t>
   </si>
   <si>
     <t xml:space="preserve">Erstimpfungen</t>
   </si>
   <si>
-    <t xml:space="preserve">45442763</t>
-  </si>
-  <si>
-    <t xml:space="preserve">45491691</t>
+    <t xml:space="preserve">45454268</t>
+  </si>
+  <si>
+    <t xml:space="preserve">45500014</t>
   </si>
   <si>
     <t xml:space="preserve">Zweitimpfungen</t>
   </si>
   <si>
-    <t xml:space="preserve">49307996</t>
-  </si>
-  <si>
-    <t xml:space="preserve">49458757</t>
+    <t xml:space="preserve">49343161</t>
+  </si>
+  <si>
+    <t xml:space="preserve">49486329</t>
   </si>
   <si>
     <t xml:space="preserve">Booster</t>
   </si>
   <si>
-    <t xml:space="preserve">29287946</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29656368</t>
+    <t xml:space="preserve">29377762</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29738164</t>
   </si>
   <si>
     <t xml:space="preserve">2. Booster</t>
   </si>
   <si>
+    <t xml:space="preserve">241087</t>
+  </si>
+  <si>
+    <t xml:space="preserve">398987</t>
+  </si>
+  <si>
     <t xml:space="preserve">geliefert</t>
   </si>
   <si>
@@ -408,28 +420,34 @@
     <t xml:space="preserve">Moderna</t>
   </si>
   <si>
-    <t xml:space="preserve">29082307 (17,2 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29180413 (17,1 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5091779</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5095185</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6218367</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6234872</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17772161</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17850356</t>
+    <t xml:space="preserve">29179553 (17,2 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29316501 (17,2 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5092440</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5096014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6221945</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6237755</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17789837</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17866929</t>
+  </si>
+  <si>
+    <t xml:space="preserve">75331</t>
+  </si>
+  <si>
+    <t xml:space="preserve">115803</t>
   </si>
   <si>
     <t xml:space="preserve">34752920</t>
@@ -438,28 +456,28 @@
     <t xml:space="preserve">AstraZeneca</t>
   </si>
   <si>
-    <t xml:space="preserve">12754678 ( 7,5 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12755420 ( 7,5 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9275791</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9276154</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3473710</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3473912</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5177</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5354</t>
+    <t xml:space="preserve">12754835 ( 7,5 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12755500 ( 7,5 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9275910</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9276159</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3473747</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3473923</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5178</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5418</t>
   </si>
   <si>
     <t xml:space="preserve">14438230</t>
@@ -468,27 +486,54 @@
     <t xml:space="preserve">Johnson&amp;Johnson</t>
   </si>
   <si>
-    <t xml:space="preserve">3622552 ( 2,1 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3623869 ( 2,1 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3606131</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3606939</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16421</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16930</t>
+    <t xml:space="preserve">3623559 ( 2,1 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3625455 ( 2,1 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Einzeldosis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3606291</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3607054</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16505</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17158</t>
+  </si>
+  <si>
+    <t xml:space="preserve">763</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1243</t>
   </si>
   <si>
     <t xml:space="preserve">5369615</t>
   </si>
   <si>
+    <t xml:space="preserve">Novavax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 ( 0,0 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14611 ( 0,0 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13182</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1429</t>
+  </si>
+  <si>
     <t xml:space="preserve">Testungen</t>
   </si>
   <si>
@@ -571,9 +616,6 @@
   </si>
   <si>
     <t xml:space="preserve">Neue Fälle je 100.000 EW in 7 Tagen bezogen auf die jeweilige Gruppe:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1429</t>
   </si>
   <si>
     <t xml:space="preserve">1306</t>
@@ -1641,10 +1683,14 @@
       <c r="A7" t="s">
         <v>22</v>
       </c>
-      <c r="B7"/>
-      <c r="C7"/>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
       <c r="D7" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1663,28 +1709,28 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B1" t="s">
-        <v>290</v>
+        <v>304</v>
       </c>
       <c r="C1" t="s">
-        <v>291</v>
+        <v>305</v>
       </c>
       <c r="D1" t="s">
-        <v>292</v>
+        <v>306</v>
       </c>
       <c r="E1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F1" t="s">
-        <v>218</v>
+        <v>232</v>
       </c>
       <c r="G1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H1" t="s">
-        <v>293</v>
+        <v>307</v>
       </c>
     </row>
     <row r="2">
@@ -1692,441 +1738,441 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>294</v>
+        <v>308</v>
       </c>
       <c r="C2" t="n">
         <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>295</v>
+        <v>309</v>
       </c>
       <c r="E2" t="n">
         <v>569</v>
       </c>
       <c r="F2" t="s">
-        <v>296</v>
+        <v>310</v>
       </c>
       <c r="G2" t="n">
         <v>1306</v>
       </c>
       <c r="H2" t="s">
-        <v>297</v>
+        <v>311</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>298</v>
+        <v>312</v>
       </c>
       <c r="C3" t="n">
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>295</v>
+        <v>309</v>
       </c>
       <c r="E3" t="n">
         <v>647</v>
       </c>
       <c r="F3" t="s">
-        <v>299</v>
+        <v>313</v>
       </c>
       <c r="G3" t="n">
         <v>1514</v>
       </c>
       <c r="H3" t="s">
-        <v>300</v>
+        <v>314</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>301</v>
+        <v>315</v>
       </c>
       <c r="C4" t="n">
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>302</v>
+        <v>316</v>
       </c>
       <c r="E4" t="n">
         <v>784</v>
       </c>
       <c r="F4" t="s">
-        <v>303</v>
+        <v>317</v>
       </c>
       <c r="G4" t="n">
         <v>1765</v>
       </c>
       <c r="H4" t="s">
-        <v>304</v>
+        <v>318</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B5" t="s">
-        <v>305</v>
+        <v>319</v>
       </c>
       <c r="C5" t="n">
         <v>47</v>
       </c>
       <c r="D5" t="s">
-        <v>306</v>
+        <v>320</v>
       </c>
       <c r="E5" t="n">
         <v>460</v>
       </c>
       <c r="F5" t="s">
-        <v>307</v>
+        <v>321</v>
       </c>
       <c r="G5" t="n">
         <v>1142</v>
       </c>
       <c r="H5" t="s">
-        <v>308</v>
+        <v>322</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>309</v>
+        <v>323</v>
       </c>
       <c r="C6" t="n">
         <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>310</v>
+        <v>324</v>
       </c>
       <c r="E6" t="n">
         <v>572</v>
       </c>
       <c r="F6" t="s">
-        <v>311</v>
+        <v>325</v>
       </c>
       <c r="G6" t="n">
         <v>1483</v>
       </c>
       <c r="H6" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B7" t="s">
-        <v>313</v>
+        <v>327</v>
       </c>
       <c r="C7" t="n">
         <v>42</v>
       </c>
       <c r="D7" t="s">
-        <v>314</v>
+        <v>328</v>
       </c>
       <c r="E7" t="n">
         <v>265</v>
       </c>
       <c r="F7" t="s">
-        <v>315</v>
+        <v>329</v>
       </c>
       <c r="G7" t="n">
         <v>739</v>
       </c>
       <c r="H7" t="s">
-        <v>316</v>
+        <v>330</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B8" t="s">
-        <v>298</v>
+        <v>312</v>
       </c>
       <c r="C8" t="n">
         <v>79</v>
       </c>
       <c r="D8" t="s">
-        <v>317</v>
+        <v>331</v>
       </c>
       <c r="E8" t="n">
         <v>264</v>
       </c>
       <c r="F8" t="s">
-        <v>318</v>
+        <v>332</v>
       </c>
       <c r="G8" t="n">
         <v>701</v>
       </c>
       <c r="H8" t="s">
-        <v>319</v>
+        <v>333</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B9" t="s">
-        <v>313</v>
+        <v>327</v>
       </c>
       <c r="C9" t="n">
         <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>320</v>
+        <v>334</v>
       </c>
       <c r="E9" t="n">
         <v>458</v>
       </c>
       <c r="F9" t="s">
-        <v>321</v>
+        <v>335</v>
       </c>
       <c r="G9" t="n">
         <v>975</v>
       </c>
       <c r="H9" t="s">
-        <v>322</v>
+        <v>336</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B10" t="s">
-        <v>323</v>
+        <v>337</v>
       </c>
       <c r="C10" t="n">
         <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>324</v>
+        <v>338</v>
       </c>
       <c r="E10" t="n">
         <v>677</v>
       </c>
       <c r="F10" t="s">
-        <v>325</v>
+        <v>339</v>
       </c>
       <c r="G10" t="n">
         <v>1564</v>
       </c>
       <c r="H10" t="s">
-        <v>326</v>
+        <v>340</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B11" t="s">
-        <v>327</v>
+        <v>341</v>
       </c>
       <c r="C11" t="n">
         <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>328</v>
+        <v>342</v>
       </c>
       <c r="E11" t="n">
         <v>473</v>
       </c>
       <c r="F11" t="s">
-        <v>329</v>
+        <v>343</v>
       </c>
       <c r="G11" t="n">
         <v>1220</v>
       </c>
       <c r="H11" t="s">
-        <v>330</v>
+        <v>344</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B12" t="s">
-        <v>331</v>
+        <v>345</v>
       </c>
       <c r="C12" t="n">
         <v>26</v>
       </c>
       <c r="D12" t="s">
-        <v>332</v>
+        <v>346</v>
       </c>
       <c r="E12" t="n">
         <v>532</v>
       </c>
       <c r="F12" t="s">
-        <v>333</v>
+        <v>347</v>
       </c>
       <c r="G12" t="n">
         <v>1122</v>
       </c>
       <c r="H12" t="s">
-        <v>334</v>
+        <v>348</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B13" t="s">
-        <v>335</v>
+        <v>349</v>
       </c>
       <c r="C13" t="n">
         <v>25</v>
       </c>
       <c r="D13" t="s">
-        <v>295</v>
+        <v>309</v>
       </c>
       <c r="E13" t="n">
         <v>488</v>
       </c>
       <c r="F13" t="s">
-        <v>336</v>
+        <v>350</v>
       </c>
       <c r="G13" t="n">
         <v>1052</v>
       </c>
       <c r="H13" t="s">
-        <v>337</v>
+        <v>351</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B14" t="s">
-        <v>338</v>
+        <v>352</v>
       </c>
       <c r="C14" t="n">
         <v>50</v>
       </c>
       <c r="D14" t="s">
-        <v>339</v>
+        <v>353</v>
       </c>
       <c r="E14" t="n">
         <v>689</v>
       </c>
       <c r="F14" t="s">
-        <v>340</v>
+        <v>354</v>
       </c>
       <c r="G14" t="n">
         <v>1212</v>
       </c>
       <c r="H14" t="s">
-        <v>341</v>
+        <v>355</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B15" t="s">
-        <v>342</v>
+        <v>356</v>
       </c>
       <c r="C15" t="n">
         <v>35</v>
       </c>
       <c r="D15" t="s">
-        <v>343</v>
+        <v>357</v>
       </c>
       <c r="E15" t="n">
         <v>546</v>
       </c>
       <c r="F15" t="s">
-        <v>344</v>
+        <v>358</v>
       </c>
       <c r="G15" t="n">
         <v>1337</v>
       </c>
       <c r="H15" t="s">
-        <v>326</v>
+        <v>340</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B16" t="s">
-        <v>345</v>
+        <v>359</v>
       </c>
       <c r="C16" t="n">
         <v>13</v>
       </c>
       <c r="D16" t="s">
-        <v>346</v>
+        <v>360</v>
       </c>
       <c r="E16" t="n">
         <v>781</v>
       </c>
       <c r="F16" t="s">
-        <v>347</v>
+        <v>361</v>
       </c>
       <c r="G16" t="n">
         <v>1878</v>
       </c>
       <c r="H16" t="s">
-        <v>326</v>
+        <v>340</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B17" t="s">
-        <v>348</v>
+        <v>362</v>
       </c>
       <c r="C17" t="n">
         <v>30</v>
       </c>
       <c r="D17" t="s">
-        <v>349</v>
+        <v>363</v>
       </c>
       <c r="E17" t="n">
         <v>327</v>
       </c>
       <c r="F17" t="s">
-        <v>350</v>
+        <v>364</v>
       </c>
       <c r="G17" t="n">
         <v>868</v>
       </c>
       <c r="H17" t="s">
-        <v>326</v>
+        <v>340</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B18" t="s">
-        <v>351</v>
+        <v>365</v>
       </c>
       <c r="C18" t="n">
         <v>22</v>
       </c>
       <c r="D18" t="s">
-        <v>352</v>
+        <v>366</v>
       </c>
       <c r="E18" t="n">
         <v>524</v>
       </c>
       <c r="F18" t="s">
-        <v>353</v>
+        <v>367</v>
       </c>
       <c r="G18" t="n">
         <v>1314</v>
       </c>
       <c r="H18" t="s">
-        <v>326</v>
+        <v>340</v>
       </c>
     </row>
   </sheetData>
@@ -2145,354 +2191,354 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>354</v>
+        <v>368</v>
       </c>
       <c r="B1" t="s">
-        <v>355</v>
+        <v>369</v>
       </c>
       <c r="C1" t="s">
-        <v>356</v>
+        <v>370</v>
       </c>
       <c r="D1" t="s">
-        <v>357</v>
+        <v>371</v>
       </c>
       <c r="E1" t="s">
-        <v>358</v>
+        <v>372</v>
       </c>
       <c r="F1" t="s">
-        <v>359</v>
+        <v>373</v>
       </c>
       <c r="G1" t="s">
-        <v>360</v>
+        <v>374</v>
       </c>
       <c r="H1" t="s">
-        <v>361</v>
+        <v>375</v>
       </c>
       <c r="I1" t="s">
-        <v>362</v>
+        <v>376</v>
       </c>
       <c r="J1" t="s">
-        <v>363</v>
+        <v>377</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>364</v>
+        <v>378</v>
       </c>
       <c r="B2" t="s">
-        <v>365</v>
+        <v>379</v>
       </c>
       <c r="C2" t="n">
         <v>6443412</v>
       </c>
       <c r="D2" t="s">
-        <v>366</v>
+        <v>380</v>
       </c>
       <c r="E2" t="s">
-        <v>367</v>
+        <v>381</v>
       </c>
       <c r="F2" t="n">
         <v>111316</v>
       </c>
       <c r="G2" t="s">
-        <v>364</v>
+        <v>378</v>
       </c>
       <c r="H2" t="n">
         <v>3306</v>
       </c>
       <c r="I2" t="s">
-        <v>368</v>
+        <v>382</v>
       </c>
       <c r="J2" t="s">
-        <v>369</v>
+        <v>383</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>368</v>
+        <v>382</v>
       </c>
       <c r="B3" t="s">
-        <v>370</v>
+        <v>384</v>
       </c>
       <c r="C3" t="n">
         <v>22862157</v>
       </c>
       <c r="D3" t="s">
-        <v>371</v>
+        <v>385</v>
       </c>
       <c r="E3" t="s">
-        <v>372</v>
+        <v>386</v>
       </c>
       <c r="F3" t="n">
         <v>154560</v>
       </c>
       <c r="G3" t="s">
-        <v>373</v>
+        <v>387</v>
       </c>
       <c r="H3" t="n">
         <v>2784</v>
       </c>
       <c r="I3" t="s">
-        <v>366</v>
+        <v>380</v>
       </c>
       <c r="J3" t="s">
-        <v>369</v>
+        <v>383</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>374</v>
+        <v>388</v>
       </c>
       <c r="B4" t="s">
-        <v>375</v>
+        <v>389</v>
       </c>
       <c r="C4" t="n">
         <v>3574328</v>
       </c>
       <c r="D4" t="s">
-        <v>374</v>
+        <v>388</v>
       </c>
       <c r="E4" t="s">
-        <v>376</v>
+        <v>390</v>
       </c>
       <c r="F4" t="n">
         <v>38592</v>
       </c>
       <c r="G4" t="s">
-        <v>377</v>
+        <v>391</v>
       </c>
       <c r="H4" t="n">
         <v>1693</v>
       </c>
       <c r="I4" t="s">
-        <v>378</v>
+        <v>392</v>
       </c>
       <c r="J4" t="s">
-        <v>379</v>
+        <v>393</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>377</v>
+        <v>391</v>
       </c>
       <c r="B5" t="s">
-        <v>380</v>
+        <v>394</v>
       </c>
       <c r="C5" t="n">
         <v>3258409</v>
       </c>
       <c r="D5" t="s">
-        <v>378</v>
+        <v>392</v>
       </c>
       <c r="E5" t="s">
-        <v>381</v>
+        <v>395</v>
       </c>
       <c r="F5" t="n">
         <v>99410</v>
       </c>
       <c r="G5" t="s">
-        <v>374</v>
+        <v>388</v>
       </c>
       <c r="H5" t="n">
         <v>1666</v>
       </c>
       <c r="I5" t="s">
-        <v>374</v>
+        <v>388</v>
       </c>
       <c r="J5" t="s">
-        <v>382</v>
+        <v>396</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>383</v>
+        <v>397</v>
       </c>
       <c r="B6" t="s">
-        <v>384</v>
+        <v>398</v>
       </c>
       <c r="C6" t="n">
         <v>3544034</v>
       </c>
       <c r="D6" t="s">
-        <v>385</v>
+        <v>399</v>
       </c>
       <c r="E6" t="s">
-        <v>381</v>
+        <v>395</v>
       </c>
       <c r="F6" t="n">
         <v>161797</v>
       </c>
       <c r="G6" t="s">
-        <v>368</v>
+        <v>382</v>
       </c>
       <c r="H6" t="n">
         <v>1551</v>
       </c>
       <c r="I6" t="s">
-        <v>371</v>
+        <v>385</v>
       </c>
       <c r="J6" t="s">
-        <v>386</v>
+        <v>400</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>385</v>
+        <v>399</v>
       </c>
       <c r="B7" t="s">
-        <v>387</v>
+        <v>401</v>
       </c>
       <c r="C7" t="n">
         <v>18938546</v>
       </c>
       <c r="D7" t="s">
-        <v>383</v>
+        <v>397</v>
       </c>
       <c r="E7" t="s">
-        <v>388</v>
+        <v>402</v>
       </c>
       <c r="F7" t="n">
         <v>30121</v>
       </c>
       <c r="G7" t="s">
-        <v>371</v>
+        <v>385</v>
       </c>
       <c r="H7" t="n">
         <v>1088</v>
       </c>
       <c r="I7" t="s">
-        <v>377</v>
+        <v>391</v>
       </c>
       <c r="J7" t="s">
-        <v>389</v>
+        <v>403</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>378</v>
+        <v>392</v>
       </c>
       <c r="B8" t="s">
-        <v>390</v>
+        <v>404</v>
       </c>
       <c r="C8" t="n">
         <v>10977524</v>
       </c>
       <c r="D8" t="s">
-        <v>373</v>
+        <v>387</v>
       </c>
       <c r="E8" t="s">
-        <v>388</v>
+        <v>402</v>
       </c>
       <c r="F8" t="n">
         <v>122713</v>
       </c>
       <c r="G8" t="s">
-        <v>383</v>
+        <v>397</v>
       </c>
       <c r="H8" t="n">
         <v>1066</v>
       </c>
       <c r="I8" t="s">
-        <v>383</v>
+        <v>397</v>
       </c>
       <c r="J8" t="s">
-        <v>391</v>
+        <v>405</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>371</v>
+        <v>385</v>
       </c>
       <c r="B9" t="s">
-        <v>392</v>
+        <v>406</v>
       </c>
       <c r="C9" t="n">
         <v>12764558</v>
       </c>
       <c r="D9" t="s">
-        <v>377</v>
+        <v>391</v>
       </c>
       <c r="E9" t="s">
-        <v>393</v>
+        <v>407</v>
       </c>
       <c r="F9" t="n">
         <v>21039</v>
       </c>
       <c r="G9" t="s">
-        <v>378</v>
+        <v>392</v>
       </c>
       <c r="H9" t="n">
         <v>799</v>
       </c>
       <c r="I9" t="s">
-        <v>373</v>
+        <v>387</v>
       </c>
       <c r="J9" t="s">
-        <v>394</v>
+        <v>408</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>373</v>
+        <v>387</v>
       </c>
       <c r="B10" t="s">
-        <v>395</v>
+        <v>409</v>
       </c>
       <c r="C10" t="n">
         <v>14779825</v>
       </c>
       <c r="D10" t="s">
-        <v>368</v>
+        <v>382</v>
       </c>
       <c r="E10" t="s">
-        <v>393</v>
+        <v>407</v>
       </c>
       <c r="F10" t="n">
         <v>139149</v>
       </c>
       <c r="G10" t="s">
-        <v>385</v>
+        <v>399</v>
       </c>
       <c r="H10" t="n">
         <v>748</v>
       </c>
       <c r="I10" t="s">
-        <v>385</v>
+        <v>399</v>
       </c>
       <c r="J10" t="s">
-        <v>396</v>
+        <v>410</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>366</v>
+        <v>380</v>
       </c>
       <c r="B11" t="s">
-        <v>397</v>
+        <v>411</v>
       </c>
       <c r="C11" t="n">
         <v>5660493</v>
       </c>
       <c r="D11" t="s">
-        <v>364</v>
+        <v>378</v>
       </c>
       <c r="E11" t="s">
-        <v>398</v>
+        <v>412</v>
       </c>
       <c r="F11" t="n">
         <v>22109</v>
       </c>
       <c r="G11" t="s">
-        <v>366</v>
+        <v>380</v>
       </c>
       <c r="H11" t="n">
         <v>683</v>
       </c>
       <c r="I11" t="s">
-        <v>364</v>
+        <v>378</v>
       </c>
       <c r="J11" t="s">
-        <v>399</v>
+        <v>413</v>
       </c>
     </row>
   </sheetData>
@@ -2511,30 +2557,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3">
@@ -2542,41 +2588,41 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -2595,25 +2641,25 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2">
@@ -2624,13 +2670,13 @@
         <v>675625</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F2" t="n">
         <v>1196</v>
@@ -2641,19 +2687,19 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B3" t="n">
         <v>64045</v>
       </c>
       <c r="C3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F3" t="n">
         <v>1368</v>
@@ -2664,19 +2710,19 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B4" t="n">
         <v>71972</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D4" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E4" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F4" t="n">
         <v>1582</v>
@@ -2687,19 +2733,19 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B5" t="n">
         <v>25975</v>
       </c>
       <c r="C5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="F5" t="n">
         <v>900</v>
@@ -2710,19 +2756,19 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B6" t="n">
         <v>19981</v>
       </c>
       <c r="C6" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E6" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F6" t="n">
         <v>1435</v>
@@ -2733,19 +2779,19 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B7" t="n">
         <v>5448</v>
       </c>
       <c r="C7" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D7" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E7" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F7" t="n">
         <v>648</v>
@@ -2756,19 +2802,19 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B8" t="n">
         <v>62794</v>
       </c>
       <c r="C8" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D8" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E8" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="F8" t="n">
         <v>540</v>
@@ -2779,19 +2825,19 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B9" t="n">
         <v>43131</v>
       </c>
       <c r="C9" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D9" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E9" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="F9" t="n">
         <v>877</v>
@@ -2802,19 +2848,19 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B10" t="n">
         <v>14589</v>
       </c>
       <c r="C10" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D10" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="E10" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="F10" t="n">
         <v>1679</v>
@@ -2825,19 +2871,19 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B11" t="n">
         <v>73865</v>
       </c>
       <c r="C11" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D11" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="E11" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F11" t="n">
         <v>1150</v>
@@ -2848,19 +2894,19 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B12" t="n">
         <v>166814</v>
       </c>
       <c r="C12" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D12" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E12" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F12" t="n">
         <v>1005</v>
@@ -2871,19 +2917,19 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B13" t="n">
         <v>26277</v>
       </c>
       <c r="C13" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D13" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E13" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F13" t="n">
         <v>985</v>
@@ -2894,19 +2940,19 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B14" t="n">
         <v>6010</v>
       </c>
       <c r="C14" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D14" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E14" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F14" t="n">
         <v>1295</v>
@@ -2917,19 +2963,19 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B15" t="n">
         <v>19707</v>
       </c>
       <c r="C15" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D15" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E15" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="F15" t="n">
         <v>1260</v>
@@ -2940,19 +2986,19 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B16" t="n">
         <v>20582</v>
       </c>
       <c r="C16" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D16" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E16" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="F16" t="n">
         <v>1677</v>
@@ -2963,19 +3009,19 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B17" t="n">
         <v>38469</v>
       </c>
       <c r="C17" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D17" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E17" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F17" t="n">
         <v>956</v>
@@ -2986,19 +3032,19 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B18" t="n">
         <v>15966</v>
       </c>
       <c r="C18" t="s">
-        <v>62</v>
+        <v>109</v>
       </c>
       <c r="D18" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="E18" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="F18" t="n">
         <v>1336</v>
@@ -3023,251 +3069,307 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B3" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C3" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B4" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C4" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B5" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C5" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>124</v>
-      </c>
-      <c r="B6"/>
-      <c r="C6"/>
+        <v>126</v>
+      </c>
+      <c r="B6" t="s">
+        <v>127</v>
+      </c>
+      <c r="C6" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="B7" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="C7" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B8" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="C8" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B9" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C9" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B10" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="C10" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B11" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="C11" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>124</v>
-      </c>
-      <c r="B12"/>
-      <c r="C12"/>
+        <v>126</v>
+      </c>
+      <c r="B12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C12" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="B13" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="C13" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="B14" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="C14" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B15" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="C15" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B16" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="C16" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B17" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="C17" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="B18" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C18" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="B19" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="C19" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>115</v>
-      </c>
-      <c r="B20"/>
-      <c r="C20"/>
+        <v>156</v>
+      </c>
+      <c r="B20" t="s">
+        <v>157</v>
+      </c>
+      <c r="C20" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="B21" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="C21" t="s">
-        <v>151</v>
+        <v>160</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="B22" t="s">
-        <v>152</v>
+        <v>161</v>
       </c>
       <c r="C22" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>124</v>
-      </c>
-      <c r="B23"/>
-      <c r="C23"/>
+        <v>129</v>
+      </c>
+      <c r="B23" t="s">
+        <v>163</v>
+      </c>
+      <c r="C23" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>125</v>
+        <v>164</v>
       </c>
       <c r="B24" t="s">
-        <v>154</v>
+        <v>165</v>
       </c>
       <c r="C24" t="s">
-        <v>154</v>
-      </c>
+        <v>166</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>117</v>
+      </c>
+      <c r="B25" t="s">
+        <v>167</v>
+      </c>
+      <c r="C25" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>120</v>
+      </c>
+      <c r="B26" t="s">
+        <v>167</v>
+      </c>
+      <c r="C26" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>123</v>
+      </c>
+      <c r="B27" t="s">
+        <v>167</v>
+      </c>
+      <c r="C27" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>129</v>
+      </c>
+      <c r="B28"/>
+      <c r="C28"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3285,86 +3387,86 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>155</v>
+        <v>170</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>156</v>
+        <v>171</v>
       </c>
       <c r="D1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>157</v>
+        <v>172</v>
       </c>
       <c r="B2" t="s">
-        <v>158</v>
+        <v>173</v>
       </c>
       <c r="C2" t="s">
-        <v>159</v>
+        <v>174</v>
       </c>
       <c r="D2" t="s">
-        <v>160</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>161</v>
+        <v>176</v>
       </c>
       <c r="B3" t="s">
-        <v>162</v>
+        <v>177</v>
       </c>
       <c r="C3" t="s">
-        <v>163</v>
+        <v>178</v>
       </c>
       <c r="D3" t="s">
-        <v>164</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>165</v>
+        <v>180</v>
       </c>
       <c r="B4" t="s">
-        <v>166</v>
+        <v>181</v>
       </c>
       <c r="C4" t="s">
-        <v>167</v>
+        <v>182</v>
       </c>
       <c r="D4" t="s">
-        <v>168</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>169</v>
+        <v>184</v>
       </c>
       <c r="B5" t="s">
-        <v>170</v>
+        <v>185</v>
       </c>
       <c r="C5" t="s">
-        <v>171</v>
+        <v>186</v>
       </c>
       <c r="D5" t="s">
-        <v>172</v>
+        <v>187</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>173</v>
+        <v>188</v>
       </c>
       <c r="B6" t="s">
-        <v>174</v>
+        <v>189</v>
       </c>
       <c r="C6" t="s">
-        <v>175</v>
+        <v>190</v>
       </c>
       <c r="D6" t="s">
-        <v>176</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -3383,35 +3485,35 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>177</v>
+        <v>192</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>156</v>
+        <v>171</v>
       </c>
       <c r="D1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>178</v>
+        <v>193</v>
       </c>
       <c r="B2" t="s">
-        <v>179</v>
+        <v>194</v>
       </c>
       <c r="C2" t="s">
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="D2" t="s">
-        <v>181</v>
+        <v>196</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>182</v>
+        <v>197</v>
       </c>
       <c r="B3"/>
       <c r="C3"/>
@@ -3422,102 +3524,102 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
       <c r="C4" t="s">
-        <v>184</v>
+        <v>198</v>
       </c>
       <c r="D4" t="s">
-        <v>185</v>
+        <v>199</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>186</v>
+        <v>200</v>
       </c>
       <c r="B5" t="s">
-        <v>187</v>
+        <v>201</v>
       </c>
       <c r="C5" t="s">
-        <v>188</v>
+        <v>202</v>
       </c>
       <c r="D5" t="s">
-        <v>189</v>
+        <v>203</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>190</v>
+        <v>204</v>
       </c>
       <c r="B6" t="s">
-        <v>191</v>
+        <v>205</v>
       </c>
       <c r="C6" t="s">
-        <v>192</v>
+        <v>206</v>
       </c>
       <c r="D6" t="s">
-        <v>193</v>
+        <v>207</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>194</v>
+        <v>208</v>
       </c>
       <c r="B7" t="s">
-        <v>195</v>
+        <v>209</v>
       </c>
       <c r="C7" t="s">
-        <v>196</v>
+        <v>210</v>
       </c>
       <c r="D7" t="s">
-        <v>197</v>
+        <v>211</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>198</v>
+        <v>212</v>
       </c>
       <c r="B8" t="s">
-        <v>199</v>
+        <v>213</v>
       </c>
       <c r="C8" t="s">
-        <v>200</v>
+        <v>214</v>
       </c>
       <c r="D8" t="s">
-        <v>201</v>
+        <v>215</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>202</v>
+        <v>216</v>
       </c>
       <c r="B9" t="s">
-        <v>203</v>
+        <v>217</v>
       </c>
       <c r="C9" t="s">
-        <v>204</v>
+        <v>218</v>
       </c>
       <c r="D9" t="s">
-        <v>205</v>
+        <v>219</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>206</v>
+        <v>220</v>
       </c>
       <c r="B10" t="s">
-        <v>207</v>
+        <v>221</v>
       </c>
       <c r="C10" t="s">
-        <v>208</v>
+        <v>222</v>
       </c>
       <c r="D10" t="s">
-        <v>209</v>
+        <v>223</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>210</v>
+        <v>224</v>
       </c>
       <c r="B11"/>
       <c r="C11"/>
@@ -3528,27 +3630,27 @@
         <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>211</v>
+        <v>225</v>
       </c>
       <c r="C12" t="s">
-        <v>212</v>
+        <v>226</v>
       </c>
       <c r="D12" t="s">
-        <v>213</v>
+        <v>227</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>214</v>
+        <v>228</v>
       </c>
       <c r="B13" t="s">
-        <v>215</v>
+        <v>229</v>
       </c>
       <c r="C13" t="s">
-        <v>216</v>
+        <v>230</v>
       </c>
       <c r="D13" t="s">
-        <v>217</v>
+        <v>231</v>
       </c>
     </row>
   </sheetData>
@@ -3567,16 +3669,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>218</v>
+        <v>232</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>219</v>
+        <v>233</v>
       </c>
       <c r="D1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2">
@@ -3584,97 +3686,97 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>220</v>
+        <v>234</v>
       </c>
       <c r="C2" t="s">
-        <v>221</v>
+        <v>235</v>
       </c>
       <c r="D2" t="s">
-        <v>222</v>
+        <v>236</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>223</v>
+        <v>237</v>
       </c>
       <c r="B3" t="s">
-        <v>224</v>
+        <v>238</v>
       </c>
       <c r="C3" t="s">
-        <v>225</v>
+        <v>239</v>
       </c>
       <c r="D3" t="s">
-        <v>226</v>
+        <v>240</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>227</v>
+        <v>241</v>
       </c>
       <c r="B4" t="s">
-        <v>228</v>
+        <v>242</v>
       </c>
       <c r="C4" t="s">
-        <v>229</v>
+        <v>243</v>
       </c>
       <c r="D4" t="s">
-        <v>230</v>
+        <v>244</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>231</v>
+        <v>245</v>
       </c>
       <c r="B5" t="s">
-        <v>232</v>
+        <v>246</v>
       </c>
       <c r="C5" t="s">
-        <v>233</v>
+        <v>247</v>
       </c>
       <c r="D5" t="s">
-        <v>234</v>
+        <v>248</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>235</v>
+        <v>249</v>
       </c>
       <c r="B6" t="s">
-        <v>236</v>
+        <v>250</v>
       </c>
       <c r="C6" t="s">
-        <v>237</v>
+        <v>251</v>
       </c>
       <c r="D6" t="s">
-        <v>238</v>
+        <v>252</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>239</v>
+        <v>253</v>
       </c>
       <c r="B7" t="s">
-        <v>240</v>
+        <v>254</v>
       </c>
       <c r="C7" t="s">
-        <v>241</v>
+        <v>255</v>
       </c>
       <c r="D7" t="s">
-        <v>242</v>
+        <v>256</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>243</v>
+        <v>257</v>
       </c>
       <c r="B8" t="s">
-        <v>244</v>
+        <v>258</v>
       </c>
       <c r="C8" t="s">
-        <v>245</v>
+        <v>259</v>
       </c>
       <c r="D8" t="s">
-        <v>246</v>
+        <v>260</v>
       </c>
     </row>
   </sheetData>
@@ -3693,58 +3795,58 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>247</v>
+        <v>261</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>156</v>
+        <v>171</v>
       </c>
       <c r="D1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>248</v>
+        <v>262</v>
       </c>
       <c r="B2" t="s">
-        <v>249</v>
+        <v>263</v>
       </c>
       <c r="C2" t="s">
-        <v>250</v>
+        <v>264</v>
       </c>
       <c r="D2" t="s">
-        <v>251</v>
+        <v>265</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>252</v>
+        <v>266</v>
       </c>
       <c r="B3" t="s">
-        <v>253</v>
+        <v>267</v>
       </c>
       <c r="C3" t="s">
-        <v>254</v>
+        <v>268</v>
       </c>
       <c r="D3" t="s">
-        <v>255</v>
+        <v>269</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>256</v>
+        <v>270</v>
       </c>
       <c r="B4" t="s">
-        <v>257</v>
+        <v>271</v>
       </c>
       <c r="C4" t="s">
-        <v>258</v>
+        <v>272</v>
       </c>
       <c r="D4" t="s">
-        <v>259</v>
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -3763,58 +3865,58 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>260</v>
+        <v>274</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>261</v>
+        <v>275</v>
       </c>
       <c r="D1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>262</v>
+        <v>276</v>
       </c>
       <c r="B2" t="s">
-        <v>263</v>
+        <v>277</v>
       </c>
       <c r="C2" t="s">
-        <v>264</v>
+        <v>278</v>
       </c>
       <c r="D2" t="s">
-        <v>265</v>
+        <v>279</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>266</v>
+        <v>280</v>
       </c>
       <c r="B3" t="s">
-        <v>267</v>
+        <v>281</v>
       </c>
       <c r="C3" t="s">
-        <v>268</v>
+        <v>282</v>
       </c>
       <c r="D3" t="s">
-        <v>269</v>
+        <v>283</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>270</v>
+        <v>284</v>
       </c>
       <c r="B4" t="s">
-        <v>271</v>
+        <v>285</v>
       </c>
       <c r="C4" t="s">
-        <v>272</v>
+        <v>286</v>
       </c>
       <c r="D4" t="s">
-        <v>273</v>
+        <v>287</v>
       </c>
     </row>
     <row r="5">
@@ -3822,18 +3924,18 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>274</v>
+        <v>288</v>
       </c>
       <c r="C5" t="s">
-        <v>275</v>
+        <v>289</v>
       </c>
       <c r="D5" t="s">
-        <v>276</v>
+        <v>290</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>277</v>
+        <v>291</v>
       </c>
       <c r="B6"/>
       <c r="C6"/>
@@ -3841,44 +3943,44 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>262</v>
+        <v>276</v>
       </c>
       <c r="B7" t="s">
-        <v>278</v>
+        <v>292</v>
       </c>
       <c r="C7" t="s">
-        <v>279</v>
+        <v>293</v>
       </c>
       <c r="D7" t="s">
-        <v>280</v>
+        <v>294</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>266</v>
+        <v>280</v>
       </c>
       <c r="B8" t="s">
-        <v>281</v>
+        <v>295</v>
       </c>
       <c r="C8" t="s">
-        <v>282</v>
+        <v>296</v>
       </c>
       <c r="D8" t="s">
-        <v>283</v>
+        <v>297</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>270</v>
+        <v>284</v>
       </c>
       <c r="B9" t="s">
-        <v>284</v>
+        <v>298</v>
       </c>
       <c r="C9" t="s">
-        <v>285</v>
+        <v>299</v>
       </c>
       <c r="D9" t="s">
-        <v>286</v>
+        <v>300</v>
       </c>
     </row>
     <row r="10">
@@ -3886,13 +3988,13 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>287</v>
+        <v>301</v>
       </c>
       <c r="C10" t="s">
-        <v>288</v>
+        <v>302</v>
       </c>
       <c r="D10" t="s">
-        <v>289</v>
+        <v>303</v>
       </c>
     </row>
   </sheetData>

</xml_diff>